<commit_message>
aparte directory voor voorbeelden niet gereerd
</commit_message>
<xml_diff>
--- a/1.0.4/matrix/Validatiematrix v1.2.xlsx
+++ b/1.0.4/matrix/Validatiematrix v1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDA0216-4955-4F90-8581-9C294E7D5167}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7866B167-7543-41F5-B6FC-9790671F5796}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9519" uniqueCount="1788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9520" uniqueCount="1788">
   <si>
     <t>Is Opdracht.zip een geldige zip</t>
   </si>
@@ -6077,7 +6077,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -6329,6 +6329,9 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="8">
     <cellStyle name="Normal 2" xfId="4" xr:uid="{0EC6E668-CD22-429A-B10D-9E4834C96B63}"/>
@@ -6340,7 +6343,47 @@
     <cellStyle name="Standaard 3 2" xfId="3" xr:uid="{A1634239-92B9-4583-AB04-DEBDF9A9A44B}"/>
     <cellStyle name="Standaard 3 3" xfId="5" xr:uid="{C77AD319-D6C6-4ABD-AE5A-A2C0A40B68E7}"/>
   </cellStyles>
-  <dxfs count="228">
+  <dxfs count="232">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -8990,7 +9033,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B125" sqref="B125"/>
+      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -14980,11 +15023,11 @@
       </c>
     </row>
     <row r="125" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="70" t="s">
+      <c r="A125" s="84" t="s">
         <v>1169</v>
       </c>
-      <c r="B125" s="74">
-        <v>2</v>
+      <c r="B125" s="81" t="s">
+        <v>1779</v>
       </c>
       <c r="C125" s="40" t="s">
         <v>1281</v>
@@ -41260,1123 +41303,1143 @@
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="F335:F339 C111:C115 F397:F408 F322:F333 F201 F269:F271 F267 F265 F259:F260 F223:F225 F219:F220 F214:F216 F203:F205 F291:G291 E450 H400:N408 G322:N339 E444:N445 M468:N475 B41:C53 B57:C62 B93:C95 B131:C138 M113:N116 G131:G138 M131:N138 B74:C81 M197:N197 G197 M41:N49 M51:N53 M57:N63 M74:N80 M88:N90 M93:N95 G51:G53 G57:G63 G74:G80 G88:G90 G93:G95 M577:N592 B66:C68 G66:G68 M66:N68 B109:C110 G108:G116 M108:N111 B148:C154 B83:C90 G84:G86 M84:N86 C116:D123 B144:C145 M144:N145 G144:G145 H155:N168 M148:N168 G148:G168 G201:N206 M451:N454 G505:G514 M504:N514 F208:N210 F212 F227:F230 G212:N230 G257:N260 F257 G118:G122 M118:N122 C126:D128 F370:F373 F346:G349 H346:N366 G370:G375 G385:G408 M596:N639 H370:N378 H385:N396 G39:G49 G37 A2:A3 B70:C70 M70:N70 G70 B1:O1 A126:B138 A140:B141 A144:B171 A197:B250 A255:B260 A262:B514 G262:N276 F262:F263 M641:N670 A37:B37 A25:A36 M5:N19 G5:G19 A516:B670 A515 M516:N575 G516:G670 A5:C24 A39:B62 A64:B68 A70:B90 A92:B107 A109:B118 A120:B124">
-    <cfRule type="containsText" dxfId="15" priority="382" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="19" priority="386" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B297:B305 B201:B206 B208:B250">
-    <cfRule type="containsText" dxfId="227" priority="477" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="231" priority="481" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B201)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F394:F396">
-    <cfRule type="containsText" dxfId="226" priority="467" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="230" priority="471" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F394)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H290:N290">
-    <cfRule type="containsText" dxfId="225" priority="475" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="229" priority="479" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H290)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M444:N445">
-    <cfRule type="containsText" dxfId="224" priority="466" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="228" priority="470" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H445:L445">
-    <cfRule type="containsText" dxfId="223" priority="465" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="227" priority="469" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G445:L445">
-    <cfRule type="containsText" dxfId="222" priority="464" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="226" priority="468" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M445:N445">
-    <cfRule type="containsText" dxfId="221" priority="462" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="225" priority="466" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H444:L444">
-    <cfRule type="containsText" dxfId="220" priority="461" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="224" priority="465" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G444:L444">
-    <cfRule type="containsText" dxfId="219" priority="460" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="223" priority="464" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M444:N444">
-    <cfRule type="containsText" dxfId="218" priority="458" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="222" priority="462" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F334">
-    <cfRule type="containsText" dxfId="217" priority="457" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="221" priority="461" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F334)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F374:F378 F385:F393">
-    <cfRule type="containsText" dxfId="216" priority="456" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="220" priority="460" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F374)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H397:N398">
-    <cfRule type="containsText" dxfId="215" priority="455" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="219" priority="459" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H397)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M455">
-    <cfRule type="containsText" dxfId="214" priority="424" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="218" priority="428" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H450:N450">
-    <cfRule type="containsText" dxfId="213" priority="450" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="217" priority="454" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N467">
-    <cfRule type="containsText" dxfId="212" priority="410" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="216" priority="414" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H399:N399">
-    <cfRule type="containsText" dxfId="211" priority="393" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="215" priority="397" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H399)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B466">
-    <cfRule type="containsText" dxfId="210" priority="441" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="214" priority="445" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M467">
-    <cfRule type="containsText" dxfId="209" priority="412" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="213" priority="416" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G456">
-    <cfRule type="containsText" dxfId="208" priority="427" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="212" priority="431" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M466">
-    <cfRule type="containsText" dxfId="207" priority="416" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="211" priority="420" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N455">
-    <cfRule type="containsText" dxfId="206" priority="422" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="210" priority="426" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B455:B465">
-    <cfRule type="containsText" dxfId="205" priority="440" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="209" priority="444" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N466">
-    <cfRule type="containsText" dxfId="204" priority="414" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="208" priority="418" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M456">
-    <cfRule type="containsText" dxfId="203" priority="420" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="207" priority="424" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N456">
-    <cfRule type="containsText" dxfId="202" priority="418" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="206" priority="422" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P342:X345">
-    <cfRule type="containsText" dxfId="201" priority="381" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="205" priority="385" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E342:F342 E344:F345">
-    <cfRule type="containsText" dxfId="200" priority="380" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="204" priority="384" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H344:H345">
-    <cfRule type="containsText" dxfId="199" priority="379" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="203" priority="383" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H344)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I342 I344:I345">
-    <cfRule type="containsText" dxfId="198" priority="378" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="202" priority="382" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J342 J344:J345">
-    <cfRule type="containsText" dxfId="197" priority="377" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="201" priority="381" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K342 K344:K345">
-    <cfRule type="containsText" dxfId="196" priority="376" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="200" priority="380" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L342 L344:L345">
-    <cfRule type="containsText" dxfId="195" priority="375" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="199" priority="379" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M342 M344:M345">
-    <cfRule type="containsText" dxfId="194" priority="374" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="198" priority="378" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N342 N344:N345">
-    <cfRule type="containsText" dxfId="193" priority="373" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="197" priority="377" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P409:X409">
-    <cfRule type="containsText" dxfId="192" priority="372" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="196" priority="376" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F409">
-    <cfRule type="containsText" dxfId="191" priority="371" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="195" priority="375" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I409">
-    <cfRule type="containsText" dxfId="190" priority="369" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="194" priority="373" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J409">
-    <cfRule type="containsText" dxfId="189" priority="368" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="193" priority="372" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K409">
-    <cfRule type="containsText" dxfId="188" priority="367" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="192" priority="371" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L409">
-    <cfRule type="containsText" dxfId="187" priority="366" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="191" priority="370" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M409">
-    <cfRule type="containsText" dxfId="186" priority="365" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="190" priority="369" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N409">
-    <cfRule type="containsText" dxfId="185" priority="364" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="189" priority="368" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B505:B513">
-    <cfRule type="containsText" dxfId="184" priority="362" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="188" priority="366" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B505)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B514">
-    <cfRule type="containsText" dxfId="183" priority="341" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="187" priority="345" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B514)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111:B114">
-    <cfRule type="containsText" dxfId="182" priority="329" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="186" priority="333" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B111)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B306 B296">
-    <cfRule type="containsText" dxfId="181" priority="330" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="185" priority="334" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B467:B475">
-    <cfRule type="containsText" dxfId="180" priority="327" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="184" priority="331" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B307:B321">
-    <cfRule type="containsText" dxfId="179" priority="328" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="183" priority="332" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B307)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B516">
-    <cfRule type="containsText" dxfId="178" priority="326" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="182" priority="330" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B516)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B450">
-    <cfRule type="containsText" dxfId="177" priority="324" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="181" priority="328" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B449">
-    <cfRule type="containsText" dxfId="176" priority="323" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="180" priority="327" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B322:B448">
-    <cfRule type="containsText" dxfId="175" priority="322" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="179" priority="326" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B322)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G504">
-    <cfRule type="containsText" dxfId="174" priority="302" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="178" priority="306" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G504)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37 C39:C40">
-    <cfRule type="containsText" dxfId="173" priority="297" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="177" priority="301" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E409">
-    <cfRule type="containsText" dxfId="172" priority="295" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="176" priority="299" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M112:N112">
-    <cfRule type="containsText" dxfId="171" priority="288" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="175" priority="292" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:D71">
-    <cfRule type="containsText" dxfId="170" priority="283" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="174" priority="287" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:D92">
-    <cfRule type="containsText" dxfId="169" priority="281" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="173" priority="285" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C129:D130">
-    <cfRule type="containsText" dxfId="168" priority="256" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="172" priority="260" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C129)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G126:G130 M126:N130">
-    <cfRule type="containsText" dxfId="167" priority="255" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="171" priority="259" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B169:B171">
-    <cfRule type="containsText" dxfId="166" priority="254" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="170" priority="258" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G169:G170">
-    <cfRule type="containsText" dxfId="165" priority="253" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="169" priority="257" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H169:N170">
-    <cfRule type="containsText" dxfId="164" priority="252" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="168" priority="256" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M446:N449 M438:N443 M420:N427 M92:N92 M87:N87 M71:N71 M54:N56 M50:N50 M37:N37 M39:N40">
-    <cfRule type="containsText" dxfId="163" priority="250" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="167" priority="254" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M65:N65 G65">
-    <cfRule type="containsText" dxfId="162" priority="245" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="166" priority="249" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64:B65">
-    <cfRule type="containsText" dxfId="161" priority="247" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="165" priority="251" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M64:N64 G64">
-    <cfRule type="containsText" dxfId="160" priority="246" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="164" priority="250" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:B73">
-    <cfRule type="containsText" dxfId="159" priority="241" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="163" priority="245" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M72:N72">
-    <cfRule type="containsText" dxfId="158" priority="243" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="162" priority="247" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M73:N73">
-    <cfRule type="containsText" dxfId="157" priority="242" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="161" priority="246" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96:D107">
-    <cfRule type="containsText" dxfId="156" priority="238" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="160" priority="242" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M96:N107 G96:G107">
-    <cfRule type="containsText" dxfId="155" priority="239" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="159" priority="243" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M83:N83 G83">
-    <cfRule type="containsText" dxfId="154" priority="224" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="158" priority="228" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M82:N82 G82">
-    <cfRule type="containsText" dxfId="153" priority="223" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="157" priority="227" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:N207">
-    <cfRule type="containsText" dxfId="152" priority="231" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="156" priority="235" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B146:B147">
-    <cfRule type="containsText" dxfId="151" priority="233" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="155" priority="237" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G146:G147 M146:N147">
-    <cfRule type="containsText" dxfId="150" priority="232" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="154" priority="236" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="containsText" dxfId="149" priority="225" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="153" priority="229" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G123 M123:N123">
-    <cfRule type="containsText" dxfId="148" priority="222" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="152" priority="226" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:B141">
-    <cfRule type="containsText" dxfId="147" priority="219" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="151" priority="223" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G140:G141 M140:N141">
-    <cfRule type="containsText" dxfId="146" priority="218" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="150" priority="222" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B198:B200">
-    <cfRule type="containsText" dxfId="145" priority="169" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="149" priority="173" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B198)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M198:N200 G198:G200">
-    <cfRule type="containsText" dxfId="144" priority="168" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="148" priority="172" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G198)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B255:B258">
-    <cfRule type="containsText" dxfId="143" priority="158" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="147" priority="162" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B517:B546">
-    <cfRule type="containsText" dxfId="142" priority="155" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="146" priority="159" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B517)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="containsText" dxfId="141" priority="153" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="145" priority="157" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H171:N171">
-    <cfRule type="containsText" dxfId="140" priority="149" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="144" priority="153" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H171)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F211:N211">
-    <cfRule type="containsText" dxfId="139" priority="147" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="143" priority="151" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171">
-    <cfRule type="containsText" dxfId="138" priority="150" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="142" priority="154" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G171)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F231:N249 F255:N256">
-    <cfRule type="containsText" dxfId="137" priority="144" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="141" priority="148" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117:N117 G117">
-    <cfRule type="containsText" dxfId="136" priority="143" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="140" priority="147" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124:D124">
-    <cfRule type="containsText" dxfId="135" priority="142" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="139" priority="146" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G124 M124:N124">
-    <cfRule type="containsText" dxfId="134" priority="141" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="138" priority="145" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F250:N250">
-    <cfRule type="containsText" dxfId="133" priority="140" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="137" priority="144" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="132" priority="139" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="136" priority="143" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G342">
-    <cfRule type="containsText" dxfId="131" priority="137" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="135" priority="141" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H342">
-    <cfRule type="containsText" dxfId="130" priority="136" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="134" priority="140" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F340">
-    <cfRule type="containsText" dxfId="129" priority="135" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="133" priority="139" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F350:F366">
-    <cfRule type="containsText" dxfId="128" priority="134" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="132" priority="138" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F350)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I340">
-    <cfRule type="containsText" dxfId="127" priority="133" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="131" priority="137" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J340">
-    <cfRule type="containsText" dxfId="126" priority="132" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="130" priority="136" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K340">
-    <cfRule type="containsText" dxfId="125" priority="131" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="129" priority="135" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L340">
-    <cfRule type="containsText" dxfId="124" priority="130" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="128" priority="134" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M340">
-    <cfRule type="containsText" dxfId="123" priority="129" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="127" priority="133" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N340">
-    <cfRule type="containsText" dxfId="122" priority="128" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="126" priority="132" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H340">
-    <cfRule type="containsText" dxfId="121" priority="127" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="125" priority="131" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G24 M20:N24">
-    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="124" priority="127" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G457:G465">
-    <cfRule type="containsText" dxfId="119" priority="122" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M457:M465">
-    <cfRule type="containsText" dxfId="118" priority="121" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="122" priority="125" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N457:N465">
-    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="121" priority="124" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M593:N593">
-    <cfRule type="containsText" dxfId="116" priority="119" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M593)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M594:N594">
-    <cfRule type="containsText" dxfId="115" priority="118" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="119" priority="122" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M594)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F341">
-    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="118" priority="121" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I341">
-    <cfRule type="containsText" dxfId="113" priority="116" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J341">
-    <cfRule type="containsText" dxfId="112" priority="115" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="116" priority="119" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K341">
-    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="115" priority="118" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L341">
-    <cfRule type="containsText" dxfId="110" priority="113" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M341">
-    <cfRule type="containsText" dxfId="109" priority="112" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="113" priority="116" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N341">
-    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="112" priority="115" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H341">
-    <cfRule type="containsText" dxfId="107" priority="110" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E343:F343">
-    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="110" priority="113" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I343">
-    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="109" priority="112" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J343">
-    <cfRule type="containsText" dxfId="104" priority="107" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K343">
-    <cfRule type="containsText" dxfId="103" priority="106" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="107" priority="110" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L343">
-    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M343">
-    <cfRule type="containsText" dxfId="101" priority="104" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N343">
-    <cfRule type="containsText" dxfId="100" priority="103" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="104" priority="107" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G343">
-    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="103" priority="106" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H343">
-    <cfRule type="containsText" dxfId="98" priority="101" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H367:N367">
-    <cfRule type="containsText" dxfId="97" priority="100" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="101" priority="104" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H367)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F367">
-    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="100" priority="103" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F367)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H368:N368">
-    <cfRule type="containsText" dxfId="95" priority="98" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H368)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F368">
-    <cfRule type="containsText" dxfId="94" priority="97" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="98" priority="101" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F368)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H369:N369">
-    <cfRule type="containsText" dxfId="93" priority="96" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="97" priority="100" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H369)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F369">
-    <cfRule type="containsText" dxfId="92" priority="95" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F369)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H379:N379">
-    <cfRule type="containsText" dxfId="91" priority="93" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="95" priority="97" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H379)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F379">
-    <cfRule type="containsText" dxfId="90" priority="94" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F379)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H380:N384">
-    <cfRule type="containsText" dxfId="89" priority="91" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="93" priority="95" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H380)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F380:F384">
-    <cfRule type="containsText" dxfId="88" priority="92" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="92" priority="96" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F380)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38:N38 G38 A38:C38">
-    <cfRule type="containsText" dxfId="87" priority="90" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="91" priority="94" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139:N139">
-    <cfRule type="containsText" dxfId="86" priority="85" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="90" priority="89" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A139)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A125:N125">
-    <cfRule type="containsText" dxfId="85" priority="86" operator="containsText" text="&lt;?&gt;">
+  <conditionalFormatting sqref="A125 C125:N125">
+    <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:N143">
-    <cfRule type="containsText" dxfId="84" priority="84" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172:A176 C172:N176">
-    <cfRule type="containsText" dxfId="83" priority="83" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A177:A196 C177:N196">
-    <cfRule type="containsText" dxfId="82" priority="82" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="86" priority="86" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A177)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A251:N254">
-    <cfRule type="containsText" dxfId="81" priority="81" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="85" priority="85" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M640:N640">
-    <cfRule type="containsText" dxfId="80" priority="32" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="84" priority="36" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M640)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A261 H261:N261 C261:F261">
-    <cfRule type="containsText" dxfId="79" priority="79" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="83" priority="83" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G447">
-    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="82" priority="81" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G447)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G447">
-    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="81" priority="82" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G447)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G448">
-    <cfRule type="containsText" dxfId="76" priority="75" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G448)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G448">
-    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G448)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G449">
-    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G449">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G450">
-    <cfRule type="containsText" dxfId="72" priority="71" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="76" priority="75" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G450">
-    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G451">
-    <cfRule type="containsText" dxfId="70" priority="69" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G451)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G451">
-    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G451)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G452">
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="72" priority="71" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G452)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G452">
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G452)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G453">
-    <cfRule type="containsText" dxfId="66" priority="65" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="70" priority="69" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G453)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G453">
-    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G453)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G454">
-    <cfRule type="containsText" dxfId="64" priority="63" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G454)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G454">
-    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G454)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G455">
-    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="66" priority="65" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G455">
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G466">
-    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="64" priority="63" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G466">
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G467">
-    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G467">
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G468">
-    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G468)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G468">
-    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G468)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G469">
-    <cfRule type="containsText" dxfId="54" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G469)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G469">
-    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G469)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G470">
-    <cfRule type="containsText" dxfId="52" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G470)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G470">
-    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G470)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G471">
-    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="54" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G471)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G471">
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G471)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G472">
-    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="52" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G472)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G472">
-    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G472)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G473">
-    <cfRule type="containsText" dxfId="46" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G473)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G473">
-    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G473)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G474">
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G474)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G474">
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G474)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G475">
-    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="46" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G475)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G475">
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G475)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G476">
-    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G476)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G476">
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G476)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G477">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G477)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G477">
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G477)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G478">
-    <cfRule type="containsText" dxfId="36" priority="35" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G478)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G478">
-    <cfRule type="containsText" dxfId="35" priority="36" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G478)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G479">
-    <cfRule type="containsText" dxfId="34" priority="33" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G479)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G479">
-    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G479)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:G36 G25:G28 B25:C36 M25:N36">
-    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:G30">
-    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4 M4:N4 A4:C4">
-    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O90 O92:O670">
-    <cfRule type="containsText" dxfId="29" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="33" priority="29" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G3 B2:C3 M2:N3">
-    <cfRule type="containsText" dxfId="28" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261">
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="31" priority="28" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:G91 O91">
-    <cfRule type="containsText" dxfId="26" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B261">
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B515">
-    <cfRule type="containsText" dxfId="24" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B515)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M515:N515 G515">
-    <cfRule type="containsText" dxfId="23" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G515)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:B196">
-    <cfRule type="containsText" dxfId="22" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:B196">
-    <cfRule type="containsText" dxfId="21" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="containsText" dxfId="16" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108:B108">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108:C108">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B110">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B114)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A119:B119">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B119">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45477,7 +45540,7 @@
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{AF62FD2E-052D-40DF-8032-68688A8C1623}"/>
   <conditionalFormatting sqref="A2:B479">
-    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45807,12 +45870,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 C1 A2:C37 A39:C1048576">
-    <cfRule type="containsText" dxfId="19" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38">
-    <cfRule type="containsText" dxfId="18" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
verwijderen gevalideerde 1.0.3 bestanden
</commit_message>
<xml_diff>
--- a/1.0.4/matrix/Validatiematrix v1.2.xlsx
+++ b/1.0.4/matrix/Validatiematrix v1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7866B167-7543-41F5-B6FC-9790671F5796}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E3401F-9AB1-467E-A077-14CF3EA8DDE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9520" uniqueCount="1788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9521" uniqueCount="1788">
   <si>
     <t>Is Opdracht.zip een geldige zip</t>
   </si>
@@ -6343,7 +6343,37 @@
     <cellStyle name="Standaard 3 2" xfId="3" xr:uid="{A1634239-92B9-4583-AB04-DEBDF9A9A44B}"/>
     <cellStyle name="Standaard 3 3" xfId="5" xr:uid="{C77AD319-D6C6-4ABD-AE5A-A2C0A40B68E7}"/>
   </cellStyles>
-  <dxfs count="232">
+  <dxfs count="235">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -9032,8 +9062,8 @@
   <dimension ref="A1:O670"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A126" sqref="A126"/>
+      <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B126" sqref="B126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15072,11 +15102,11 @@
       </c>
     </row>
     <row r="126" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A126" s="38" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B126" s="38">
-        <v>2</v>
+      <c r="A126" s="76" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B126" s="81" t="s">
+        <v>1779</v>
       </c>
       <c r="C126" s="18" t="s">
         <v>88</v>
@@ -41302,1124 +41332,1139 @@
     </filterColumn>
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="F335:F339 C111:C115 F397:F408 F322:F333 F201 F269:F271 F267 F265 F259:F260 F223:F225 F219:F220 F214:F216 F203:F205 F291:G291 E450 H400:N408 G322:N339 E444:N445 M468:N475 B41:C53 B57:C62 B93:C95 B131:C138 M113:N116 G131:G138 M131:N138 B74:C81 M197:N197 G197 M41:N49 M51:N53 M57:N63 M74:N80 M88:N90 M93:N95 G51:G53 G57:G63 G74:G80 G88:G90 G93:G95 M577:N592 B66:C68 G66:G68 M66:N68 B109:C110 G108:G116 M108:N111 B148:C154 B83:C90 G84:G86 M84:N86 C116:D123 B144:C145 M144:N145 G144:G145 H155:N168 M148:N168 G148:G168 G201:N206 M451:N454 G505:G514 M504:N514 F208:N210 F212 F227:F230 G212:N230 G257:N260 F257 G118:G122 M118:N122 C126:D128 F370:F373 F346:G349 H346:N366 G370:G375 G385:G408 M596:N639 H370:N378 H385:N396 G39:G49 G37 A2:A3 B70:C70 M70:N70 G70 B1:O1 A126:B138 A140:B141 A144:B171 A197:B250 A255:B260 A262:B514 G262:N276 F262:F263 M641:N670 A37:B37 A25:A36 M5:N19 G5:G19 A516:B670 A515 M516:N575 G516:G670 A5:C24 A39:B62 A64:B68 A70:B90 A92:B107 A109:B118 A120:B124">
-    <cfRule type="containsText" dxfId="19" priority="386" operator="containsText" text="&lt;?&gt;">
+  <conditionalFormatting sqref="F335:F339 C111:C115 F397:F408 F322:F333 F201 F269:F271 F267 F265 F259:F260 F223:F225 F219:F220 F214:F216 F203:F205 F291:G291 E450 H400:N408 G322:N339 E444:N445 M468:N475 B41:C53 B57:C62 B93:C95 B131:C138 M113:N116 G131:G138 M131:N138 B74:C81 M197:N197 G197 M41:N49 M51:N53 M57:N63 M74:N80 M88:N90 M93:N95 G51:G53 G57:G63 G74:G80 G88:G90 G93:G95 M577:N592 B66:C68 G66:G68 M66:N68 B109:C110 G108:G116 M108:N111 B148:C154 B83:C90 G84:G86 M84:N86 C116:D123 B144:C145 M144:N145 G144:G145 H155:N168 M148:N168 G148:G168 G201:N206 M451:N454 G505:G514 M504:N514 F208:N210 F212 F227:F230 G212:N230 G257:N260 F257 G118:G122 M118:N122 C126:D128 F370:F373 F346:G349 H346:N366 G370:G375 G385:G408 M596:N639 H370:N378 H385:N396 G39:G49 G37 A2:A3 B70:C70 M70:N70 G70 B1:O1 A140:B141 A144:B171 A197:B250 A255:B260 A262:B514 G262:N276 F262:F263 M641:N670 A37:B37 A25:A36 M5:N19 G5:G19 A516:B670 A515 M516:N575 G516:G670 A5:C24 A39:B62 A64:B68 A70:B90 A92:B107 A109:B118 A120:B124 A126:B138">
+    <cfRule type="containsText" dxfId="22" priority="389" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B297:B305 B201:B206 B208:B250">
-    <cfRule type="containsText" dxfId="231" priority="481" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="234" priority="484" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B201)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F394:F396">
-    <cfRule type="containsText" dxfId="230" priority="471" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="233" priority="474" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F394)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H290:N290">
-    <cfRule type="containsText" dxfId="229" priority="479" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="232" priority="482" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H290)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M444:N445">
-    <cfRule type="containsText" dxfId="228" priority="470" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="231" priority="473" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H445:L445">
-    <cfRule type="containsText" dxfId="227" priority="469" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="230" priority="472" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G445:L445">
-    <cfRule type="containsText" dxfId="226" priority="468" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="229" priority="471" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M445:N445">
-    <cfRule type="containsText" dxfId="225" priority="466" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="228" priority="469" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H444:L444">
-    <cfRule type="containsText" dxfId="224" priority="465" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="227" priority="468" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G444:L444">
-    <cfRule type="containsText" dxfId="223" priority="464" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="226" priority="467" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M444:N444">
-    <cfRule type="containsText" dxfId="222" priority="462" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="225" priority="465" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F334">
-    <cfRule type="containsText" dxfId="221" priority="461" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="224" priority="464" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F334)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F374:F378 F385:F393">
-    <cfRule type="containsText" dxfId="220" priority="460" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="223" priority="463" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F374)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H397:N398">
-    <cfRule type="containsText" dxfId="219" priority="459" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="222" priority="462" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H397)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M455">
-    <cfRule type="containsText" dxfId="218" priority="428" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="221" priority="431" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H450:N450">
-    <cfRule type="containsText" dxfId="217" priority="454" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="220" priority="457" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N467">
-    <cfRule type="containsText" dxfId="216" priority="414" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="219" priority="417" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H399:N399">
-    <cfRule type="containsText" dxfId="215" priority="397" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="218" priority="400" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H399)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B466">
-    <cfRule type="containsText" dxfId="214" priority="445" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="217" priority="448" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M467">
-    <cfRule type="containsText" dxfId="213" priority="416" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="216" priority="419" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G456">
-    <cfRule type="containsText" dxfId="212" priority="431" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="215" priority="434" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M466">
-    <cfRule type="containsText" dxfId="211" priority="420" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="214" priority="423" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N455">
-    <cfRule type="containsText" dxfId="210" priority="426" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="213" priority="429" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B455:B465">
-    <cfRule type="containsText" dxfId="209" priority="444" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="212" priority="447" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N466">
-    <cfRule type="containsText" dxfId="208" priority="418" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="211" priority="421" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M456">
-    <cfRule type="containsText" dxfId="207" priority="424" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="210" priority="427" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N456">
-    <cfRule type="containsText" dxfId="206" priority="422" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="209" priority="425" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P342:X345">
-    <cfRule type="containsText" dxfId="205" priority="385" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="208" priority="388" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E342:F342 E344:F345">
-    <cfRule type="containsText" dxfId="204" priority="384" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="207" priority="387" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H344:H345">
-    <cfRule type="containsText" dxfId="203" priority="383" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="206" priority="386" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H344)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I342 I344:I345">
-    <cfRule type="containsText" dxfId="202" priority="382" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="205" priority="385" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J342 J344:J345">
-    <cfRule type="containsText" dxfId="201" priority="381" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="204" priority="384" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K342 K344:K345">
-    <cfRule type="containsText" dxfId="200" priority="380" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="203" priority="383" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L342 L344:L345">
-    <cfRule type="containsText" dxfId="199" priority="379" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="202" priority="382" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M342 M344:M345">
-    <cfRule type="containsText" dxfId="198" priority="378" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="201" priority="381" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N342 N344:N345">
-    <cfRule type="containsText" dxfId="197" priority="377" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="200" priority="380" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P409:X409">
-    <cfRule type="containsText" dxfId="196" priority="376" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="199" priority="379" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F409">
-    <cfRule type="containsText" dxfId="195" priority="375" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="198" priority="378" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I409">
-    <cfRule type="containsText" dxfId="194" priority="373" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="197" priority="376" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J409">
-    <cfRule type="containsText" dxfId="193" priority="372" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="196" priority="375" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K409">
-    <cfRule type="containsText" dxfId="192" priority="371" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="195" priority="374" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L409">
-    <cfRule type="containsText" dxfId="191" priority="370" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="194" priority="373" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M409">
-    <cfRule type="containsText" dxfId="190" priority="369" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="193" priority="372" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N409">
-    <cfRule type="containsText" dxfId="189" priority="368" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="192" priority="371" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B505:B513">
-    <cfRule type="containsText" dxfId="188" priority="366" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="191" priority="369" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B505)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B514">
-    <cfRule type="containsText" dxfId="187" priority="345" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="190" priority="348" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B514)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111:B114">
-    <cfRule type="containsText" dxfId="186" priority="333" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="189" priority="336" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B111)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B306 B296">
-    <cfRule type="containsText" dxfId="185" priority="334" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="188" priority="337" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B467:B475">
-    <cfRule type="containsText" dxfId="184" priority="331" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="187" priority="334" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B307:B321">
-    <cfRule type="containsText" dxfId="183" priority="332" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="186" priority="335" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B307)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B516">
-    <cfRule type="containsText" dxfId="182" priority="330" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="185" priority="333" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B516)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B450">
-    <cfRule type="containsText" dxfId="181" priority="328" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="184" priority="331" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B449">
-    <cfRule type="containsText" dxfId="180" priority="327" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="183" priority="330" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B322:B448">
-    <cfRule type="containsText" dxfId="179" priority="326" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="182" priority="329" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B322)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G504">
-    <cfRule type="containsText" dxfId="178" priority="306" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="181" priority="309" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G504)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37 C39:C40">
-    <cfRule type="containsText" dxfId="177" priority="301" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="180" priority="304" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E409">
-    <cfRule type="containsText" dxfId="176" priority="299" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="179" priority="302" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M112:N112">
-    <cfRule type="containsText" dxfId="175" priority="292" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="178" priority="295" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:D71">
-    <cfRule type="containsText" dxfId="174" priority="287" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="177" priority="290" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:D92">
-    <cfRule type="containsText" dxfId="173" priority="285" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="176" priority="288" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C129:D130">
-    <cfRule type="containsText" dxfId="172" priority="260" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="175" priority="263" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C129)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G126:G130 M126:N130">
-    <cfRule type="containsText" dxfId="171" priority="259" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="174" priority="262" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B169:B171">
-    <cfRule type="containsText" dxfId="170" priority="258" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="173" priority="261" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G169:G170">
-    <cfRule type="containsText" dxfId="169" priority="257" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="172" priority="260" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H169:N170">
-    <cfRule type="containsText" dxfId="168" priority="256" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="171" priority="259" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M446:N449 M438:N443 M420:N427 M92:N92 M87:N87 M71:N71 M54:N56 M50:N50 M37:N37 M39:N40">
-    <cfRule type="containsText" dxfId="167" priority="254" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="170" priority="257" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M65:N65 G65">
-    <cfRule type="containsText" dxfId="166" priority="249" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="169" priority="252" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64:B65">
-    <cfRule type="containsText" dxfId="165" priority="251" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="168" priority="254" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M64:N64 G64">
-    <cfRule type="containsText" dxfId="164" priority="250" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="167" priority="253" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:B73">
-    <cfRule type="containsText" dxfId="163" priority="245" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="166" priority="248" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M72:N72">
-    <cfRule type="containsText" dxfId="162" priority="247" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="165" priority="250" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M73:N73">
-    <cfRule type="containsText" dxfId="161" priority="246" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="164" priority="249" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96:D107">
-    <cfRule type="containsText" dxfId="160" priority="242" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="163" priority="245" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M96:N107 G96:G107">
-    <cfRule type="containsText" dxfId="159" priority="243" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="162" priority="246" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M83:N83 G83">
-    <cfRule type="containsText" dxfId="158" priority="228" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="161" priority="231" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M82:N82 G82">
-    <cfRule type="containsText" dxfId="157" priority="227" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="160" priority="230" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:N207">
-    <cfRule type="containsText" dxfId="156" priority="235" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="159" priority="238" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B146:B147">
-    <cfRule type="containsText" dxfId="155" priority="237" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="158" priority="240" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G146:G147 M146:N147">
-    <cfRule type="containsText" dxfId="154" priority="236" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="157" priority="239" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="containsText" dxfId="153" priority="229" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="156" priority="232" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G123 M123:N123">
-    <cfRule type="containsText" dxfId="152" priority="226" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="155" priority="229" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:B141">
-    <cfRule type="containsText" dxfId="151" priority="223" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="154" priority="226" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G140:G141 M140:N141">
-    <cfRule type="containsText" dxfId="150" priority="222" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="153" priority="225" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B198:B200">
-    <cfRule type="containsText" dxfId="149" priority="173" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="152" priority="176" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B198)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M198:N200 G198:G200">
-    <cfRule type="containsText" dxfId="148" priority="172" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="151" priority="175" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G198)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B255:B258">
-    <cfRule type="containsText" dxfId="147" priority="162" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="150" priority="165" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B517:B546">
-    <cfRule type="containsText" dxfId="146" priority="159" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="149" priority="162" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B517)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="containsText" dxfId="145" priority="157" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="148" priority="160" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H171:N171">
-    <cfRule type="containsText" dxfId="144" priority="153" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="147" priority="156" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H171)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F211:N211">
-    <cfRule type="containsText" dxfId="143" priority="151" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="146" priority="154" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171">
-    <cfRule type="containsText" dxfId="142" priority="154" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="145" priority="157" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G171)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F231:N249 F255:N256">
-    <cfRule type="containsText" dxfId="141" priority="148" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="144" priority="151" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117:N117 G117">
-    <cfRule type="containsText" dxfId="140" priority="147" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="143" priority="150" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124:D124">
-    <cfRule type="containsText" dxfId="139" priority="146" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="142" priority="149" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G124 M124:N124">
-    <cfRule type="containsText" dxfId="138" priority="145" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="141" priority="148" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F250:N250">
-    <cfRule type="containsText" dxfId="137" priority="144" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="140" priority="147" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="136" priority="143" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="139" priority="146" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G342">
-    <cfRule type="containsText" dxfId="135" priority="141" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="138" priority="144" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H342">
-    <cfRule type="containsText" dxfId="134" priority="140" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="137" priority="143" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F340">
-    <cfRule type="containsText" dxfId="133" priority="139" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="136" priority="142" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F350:F366">
-    <cfRule type="containsText" dxfId="132" priority="138" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="135" priority="141" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F350)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I340">
-    <cfRule type="containsText" dxfId="131" priority="137" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="134" priority="140" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J340">
-    <cfRule type="containsText" dxfId="130" priority="136" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="133" priority="139" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K340">
-    <cfRule type="containsText" dxfId="129" priority="135" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="132" priority="138" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L340">
-    <cfRule type="containsText" dxfId="128" priority="134" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="131" priority="137" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M340">
-    <cfRule type="containsText" dxfId="127" priority="133" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="130" priority="136" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N340">
-    <cfRule type="containsText" dxfId="126" priority="132" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="129" priority="135" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H340">
-    <cfRule type="containsText" dxfId="125" priority="131" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="128" priority="134" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G24 M20:N24">
-    <cfRule type="containsText" dxfId="124" priority="127" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="127" priority="130" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G457:G465">
-    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M457:M465">
-    <cfRule type="containsText" dxfId="122" priority="125" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="125" priority="128" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N457:N465">
-    <cfRule type="containsText" dxfId="121" priority="124" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="124" priority="127" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M593:N593">
-    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M593)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M594:N594">
-    <cfRule type="containsText" dxfId="119" priority="122" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="122" priority="125" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M594)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F341">
-    <cfRule type="containsText" dxfId="118" priority="121" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="121" priority="124" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I341">
-    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J341">
-    <cfRule type="containsText" dxfId="116" priority="119" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="119" priority="122" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K341">
-    <cfRule type="containsText" dxfId="115" priority="118" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="118" priority="121" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L341">
-    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M341">
-    <cfRule type="containsText" dxfId="113" priority="116" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="116" priority="119" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N341">
-    <cfRule type="containsText" dxfId="112" priority="115" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="115" priority="118" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H341">
-    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E343:F343">
-    <cfRule type="containsText" dxfId="110" priority="113" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="113" priority="116" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I343">
-    <cfRule type="containsText" dxfId="109" priority="112" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="112" priority="115" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J343">
-    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K343">
-    <cfRule type="containsText" dxfId="107" priority="110" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="110" priority="113" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L343">
-    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="109" priority="112" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M343">
-    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N343">
-    <cfRule type="containsText" dxfId="104" priority="107" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="107" priority="110" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G343">
-    <cfRule type="containsText" dxfId="103" priority="106" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H343">
-    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H367:N367">
-    <cfRule type="containsText" dxfId="101" priority="104" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="104" priority="107" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H367)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F367">
-    <cfRule type="containsText" dxfId="100" priority="103" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="103" priority="106" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F367)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H368:N368">
-    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H368)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F368">
-    <cfRule type="containsText" dxfId="98" priority="101" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="101" priority="104" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F368)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H369:N369">
-    <cfRule type="containsText" dxfId="97" priority="100" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="100" priority="103" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H369)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F369">
-    <cfRule type="containsText" dxfId="96" priority="99" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F369)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H379:N379">
-    <cfRule type="containsText" dxfId="95" priority="97" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="98" priority="100" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H379)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F379">
-    <cfRule type="containsText" dxfId="94" priority="98" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F379)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H380:N384">
-    <cfRule type="containsText" dxfId="93" priority="95" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="96" priority="98" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H380)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F380:F384">
-    <cfRule type="containsText" dxfId="92" priority="96" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="95" priority="99" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F380)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38:N38 G38 A38:C38">
-    <cfRule type="containsText" dxfId="91" priority="94" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="94" priority="97" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139:N139">
-    <cfRule type="containsText" dxfId="90" priority="89" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="93" priority="92" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A139)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125 C125:N125">
-    <cfRule type="containsText" dxfId="89" priority="90" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="92" priority="93" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:N143">
-    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="91" priority="91" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172:A176 C172:N176">
-    <cfRule type="containsText" dxfId="87" priority="87" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="90" priority="90" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A177:A196 C177:N196">
-    <cfRule type="containsText" dxfId="86" priority="86" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="89" priority="89" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A177)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A251:N254">
-    <cfRule type="containsText" dxfId="85" priority="85" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M640:N640">
-    <cfRule type="containsText" dxfId="84" priority="36" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="87" priority="39" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M640)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A261 H261:N261 C261:F261">
-    <cfRule type="containsText" dxfId="83" priority="83" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="86" priority="86" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G447">
-    <cfRule type="containsText" dxfId="82" priority="81" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="85" priority="84" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G447)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G447">
-    <cfRule type="containsText" dxfId="81" priority="82" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="84" priority="85" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G447)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G448">
-    <cfRule type="containsText" dxfId="80" priority="79" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G448)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G448">
-    <cfRule type="containsText" dxfId="79" priority="80" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G448)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G449">
-    <cfRule type="containsText" dxfId="78" priority="77" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="81" priority="80" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G449">
-    <cfRule type="containsText" dxfId="77" priority="78" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G450">
-    <cfRule type="containsText" dxfId="76" priority="75" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="79" priority="78" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G450">
-    <cfRule type="containsText" dxfId="75" priority="76" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G451">
-    <cfRule type="containsText" dxfId="74" priority="73" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G451)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G451">
-    <cfRule type="containsText" dxfId="73" priority="74" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G451)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G452">
-    <cfRule type="containsText" dxfId="72" priority="71" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="75" priority="74" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G452)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G452">
-    <cfRule type="containsText" dxfId="71" priority="72" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G452)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G453">
-    <cfRule type="containsText" dxfId="70" priority="69" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="73" priority="72" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G453)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G453">
-    <cfRule type="containsText" dxfId="69" priority="70" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G453)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G454">
-    <cfRule type="containsText" dxfId="68" priority="67" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G454)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G454">
-    <cfRule type="containsText" dxfId="67" priority="68" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G454)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G455">
-    <cfRule type="containsText" dxfId="66" priority="65" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="69" priority="68" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G455">
-    <cfRule type="containsText" dxfId="65" priority="66" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G466">
-    <cfRule type="containsText" dxfId="64" priority="63" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="67" priority="66" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G466">
-    <cfRule type="containsText" dxfId="63" priority="64" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G467">
-    <cfRule type="containsText" dxfId="62" priority="61" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G467">
-    <cfRule type="containsText" dxfId="61" priority="62" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G468">
-    <cfRule type="containsText" dxfId="60" priority="59" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="63" priority="62" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G468)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G468">
-    <cfRule type="containsText" dxfId="59" priority="60" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G468)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G469">
-    <cfRule type="containsText" dxfId="58" priority="57" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="61" priority="60" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G469)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G469">
-    <cfRule type="containsText" dxfId="57" priority="58" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G469)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G470">
-    <cfRule type="containsText" dxfId="56" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G470)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G470">
-    <cfRule type="containsText" dxfId="55" priority="56" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G470)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G471">
-    <cfRule type="containsText" dxfId="54" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G471)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G471">
-    <cfRule type="containsText" dxfId="53" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G471)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G472">
-    <cfRule type="containsText" dxfId="52" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G472)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G472">
-    <cfRule type="containsText" dxfId="51" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G472)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G473">
-    <cfRule type="containsText" dxfId="50" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G473)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G473">
-    <cfRule type="containsText" dxfId="49" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G473)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G474">
-    <cfRule type="containsText" dxfId="48" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="51" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G474)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G474">
-    <cfRule type="containsText" dxfId="47" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G474)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G475">
-    <cfRule type="containsText" dxfId="46" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G475)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G475">
-    <cfRule type="containsText" dxfId="45" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G475)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G476">
-    <cfRule type="containsText" dxfId="44" priority="43" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G476)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G476">
-    <cfRule type="containsText" dxfId="43" priority="44" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G476)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G477">
-    <cfRule type="containsText" dxfId="42" priority="41" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G477)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G477">
-    <cfRule type="containsText" dxfId="41" priority="42" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G477)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G478">
-    <cfRule type="containsText" dxfId="40" priority="39" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G478)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G478">
-    <cfRule type="containsText" dxfId="39" priority="40" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G478)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G479">
-    <cfRule type="containsText" dxfId="38" priority="37" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G479)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G479">
-    <cfRule type="containsText" dxfId="37" priority="38" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G479)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:G36 G25:G28 B25:C36 M25:N36">
-    <cfRule type="containsText" dxfId="36" priority="34" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:G30">
-    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4 M4:N4 A4:C4">
-    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="37" priority="34" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O90 O92:O670">
-    <cfRule type="containsText" dxfId="33" priority="29" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="36" priority="32" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G3 B2:C3 M2:N3">
-    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261">
-    <cfRule type="containsText" dxfId="31" priority="28" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:G91 O91">
-    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B261">
-    <cfRule type="containsText" dxfId="29" priority="26" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B515">
-    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="31" priority="28" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B515)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M515:N515 G515">
-    <cfRule type="containsText" dxfId="27" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G515)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:B196">
-    <cfRule type="containsText" dxfId="26" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:B196">
-    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="containsText" dxfId="20" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108:B108">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108:C108">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B110">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B114)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A119:B119">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B119">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B125">
     <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125">
@@ -42427,19 +42472,19 @@
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B125">
+  <conditionalFormatting sqref="B126">
     <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B126)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B125">
+  <conditionalFormatting sqref="B126">
     <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B126)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B125">
+  <conditionalFormatting sqref="B126">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45540,7 +45585,7 @@
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{AF62FD2E-052D-40DF-8032-68688A8C1623}"/>
   <conditionalFormatting sqref="A2:B479">
-    <cfRule type="containsText" dxfId="24" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45870,12 +45915,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 C1 A2:C37 A39:C1048576">
-    <cfRule type="containsText" dxfId="23" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38">
-    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
niet gebruikte bestanden apart zetten
</commit_message>
<xml_diff>
--- a/1.0.4/matrix/Validatiematrix v1.2.xlsx
+++ b/1.0.4/matrix/Validatiematrix v1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E3401F-9AB1-467E-A077-14CF3EA8DDE8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{655F7892-093D-4637-8279-F0AD8B6BAF91}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9521" uniqueCount="1788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9525" uniqueCount="1788">
   <si>
     <t>Is Opdracht.zip een geldige zip</t>
   </si>
@@ -6343,7 +6343,127 @@
     <cellStyle name="Standaard 3 2" xfId="3" xr:uid="{A1634239-92B9-4583-AB04-DEBDF9A9A44B}"/>
     <cellStyle name="Standaard 3 3" xfId="5" xr:uid="{C77AD319-D6C6-4ABD-AE5A-A2C0A40B68E7}"/>
   </cellStyles>
-  <dxfs count="235">
+  <dxfs count="247">
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FFFF0000"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFFF0000"/>
@@ -9063,7 +9183,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A108" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B126" sqref="B126"/>
+      <selection pane="bottomLeft" activeCell="A132" sqref="A132:B132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -15246,11 +15366,11 @@
       </c>
     </row>
     <row r="129" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="38" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B129" s="38">
-        <v>2</v>
+      <c r="A129" s="76" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B129" s="81" t="s">
+        <v>1779</v>
       </c>
       <c r="C129" s="22" t="s">
         <v>93</v>
@@ -15294,11 +15414,11 @@
       </c>
     </row>
     <row r="130" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="38" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B130" s="38">
-        <v>2</v>
+      <c r="A130" s="76" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B130" s="81" t="s">
+        <v>1779</v>
       </c>
       <c r="C130" s="22" t="s">
         <v>94</v>
@@ -15342,11 +15462,11 @@
       </c>
     </row>
     <row r="131" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A131" s="38" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B131" s="38">
-        <v>2</v>
+      <c r="A131" s="76" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B131" s="81" t="s">
+        <v>1779</v>
       </c>
       <c r="C131" s="22" t="s">
         <v>96</v>
@@ -15390,11 +15510,11 @@
       </c>
     </row>
     <row r="132" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A132" s="38" t="s">
-        <v>1166</v>
-      </c>
-      <c r="B132" s="38">
-        <v>2</v>
+      <c r="A132" s="76" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B132" s="81" t="s">
+        <v>1779</v>
       </c>
       <c r="C132" s="22" t="s">
         <v>98</v>
@@ -41333,1158 +41453,1218 @@
   </autoFilter>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="F335:F339 C111:C115 F397:F408 F322:F333 F201 F269:F271 F267 F265 F259:F260 F223:F225 F219:F220 F214:F216 F203:F205 F291:G291 E450 H400:N408 G322:N339 E444:N445 M468:N475 B41:C53 B57:C62 B93:C95 B131:C138 M113:N116 G131:G138 M131:N138 B74:C81 M197:N197 G197 M41:N49 M51:N53 M57:N63 M74:N80 M88:N90 M93:N95 G51:G53 G57:G63 G74:G80 G88:G90 G93:G95 M577:N592 B66:C68 G66:G68 M66:N68 B109:C110 G108:G116 M108:N111 B148:C154 B83:C90 G84:G86 M84:N86 C116:D123 B144:C145 M144:N145 G144:G145 H155:N168 M148:N168 G148:G168 G201:N206 M451:N454 G505:G514 M504:N514 F208:N210 F212 F227:F230 G212:N230 G257:N260 F257 G118:G122 M118:N122 C126:D128 F370:F373 F346:G349 H346:N366 G370:G375 G385:G408 M596:N639 H370:N378 H385:N396 G39:G49 G37 A2:A3 B70:C70 M70:N70 G70 B1:O1 A140:B141 A144:B171 A197:B250 A255:B260 A262:B514 G262:N276 F262:F263 M641:N670 A37:B37 A25:A36 M5:N19 G5:G19 A516:B670 A515 M516:N575 G516:G670 A5:C24 A39:B62 A64:B68 A70:B90 A92:B107 A109:B118 A120:B124 A126:B138">
-    <cfRule type="containsText" dxfId="22" priority="389" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="34" priority="401" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B297:B305 B201:B206 B208:B250">
-    <cfRule type="containsText" dxfId="234" priority="484" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="246" priority="496" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B201)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F394:F396">
-    <cfRule type="containsText" dxfId="233" priority="474" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="245" priority="486" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F394)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H290:N290">
-    <cfRule type="containsText" dxfId="232" priority="482" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="244" priority="494" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H290)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M444:N445">
-    <cfRule type="containsText" dxfId="231" priority="473" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="243" priority="485" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H445:L445">
-    <cfRule type="containsText" dxfId="230" priority="472" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="242" priority="484" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G445:L445">
-    <cfRule type="containsText" dxfId="229" priority="471" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="241" priority="483" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M445:N445">
-    <cfRule type="containsText" dxfId="228" priority="469" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="240" priority="481" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M445)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H444:L444">
-    <cfRule type="containsText" dxfId="227" priority="468" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="239" priority="480" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G444:L444">
-    <cfRule type="containsText" dxfId="226" priority="467" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="238" priority="479" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M444:N444">
-    <cfRule type="containsText" dxfId="225" priority="465" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="237" priority="477" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M444)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F334">
-    <cfRule type="containsText" dxfId="224" priority="464" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="236" priority="476" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F334)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F374:F378 F385:F393">
-    <cfRule type="containsText" dxfId="223" priority="463" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="235" priority="475" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F374)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H397:N398">
-    <cfRule type="containsText" dxfId="222" priority="462" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="234" priority="474" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H397)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M455">
-    <cfRule type="containsText" dxfId="221" priority="431" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="233" priority="443" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H450:N450">
-    <cfRule type="containsText" dxfId="220" priority="457" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="232" priority="469" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N467">
-    <cfRule type="containsText" dxfId="219" priority="417" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="231" priority="429" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H399:N399">
-    <cfRule type="containsText" dxfId="218" priority="400" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="230" priority="412" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H399)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B466">
-    <cfRule type="containsText" dxfId="217" priority="448" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="229" priority="460" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M467">
-    <cfRule type="containsText" dxfId="216" priority="419" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="228" priority="431" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G456">
-    <cfRule type="containsText" dxfId="215" priority="434" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="227" priority="446" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M466">
-    <cfRule type="containsText" dxfId="214" priority="423" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="226" priority="435" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N455">
-    <cfRule type="containsText" dxfId="213" priority="429" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="225" priority="441" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B455:B465">
-    <cfRule type="containsText" dxfId="212" priority="447" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="224" priority="459" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N466">
-    <cfRule type="containsText" dxfId="211" priority="421" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="223" priority="433" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M456">
-    <cfRule type="containsText" dxfId="210" priority="427" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="222" priority="439" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N456">
-    <cfRule type="containsText" dxfId="209" priority="425" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="221" priority="437" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N456)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P342:X345">
-    <cfRule type="containsText" dxfId="208" priority="388" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="220" priority="400" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E342:F342 E344:F345">
-    <cfRule type="containsText" dxfId="207" priority="387" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="219" priority="399" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H344:H345">
-    <cfRule type="containsText" dxfId="206" priority="386" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="218" priority="398" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H344)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I342 I344:I345">
-    <cfRule type="containsText" dxfId="205" priority="385" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="217" priority="397" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J342 J344:J345">
-    <cfRule type="containsText" dxfId="204" priority="384" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="216" priority="396" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K342 K344:K345">
-    <cfRule type="containsText" dxfId="203" priority="383" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="215" priority="395" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L342 L344:L345">
-    <cfRule type="containsText" dxfId="202" priority="382" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="214" priority="394" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M342 M344:M345">
-    <cfRule type="containsText" dxfId="201" priority="381" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="213" priority="393" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N342 N344:N345">
-    <cfRule type="containsText" dxfId="200" priority="380" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="212" priority="392" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P409:X409">
-    <cfRule type="containsText" dxfId="199" priority="379" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="211" priority="391" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",P409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F409">
-    <cfRule type="containsText" dxfId="198" priority="378" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="210" priority="390" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I409">
-    <cfRule type="containsText" dxfId="197" priority="376" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="209" priority="388" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J409">
-    <cfRule type="containsText" dxfId="196" priority="375" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="208" priority="387" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K409">
-    <cfRule type="containsText" dxfId="195" priority="374" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="207" priority="386" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L409">
-    <cfRule type="containsText" dxfId="194" priority="373" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="206" priority="385" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M409">
-    <cfRule type="containsText" dxfId="193" priority="372" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="205" priority="384" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N409">
-    <cfRule type="containsText" dxfId="192" priority="371" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="204" priority="383" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B505:B513">
-    <cfRule type="containsText" dxfId="191" priority="369" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="203" priority="381" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B505)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B514">
-    <cfRule type="containsText" dxfId="190" priority="348" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="202" priority="360" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B514)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B111:B114">
-    <cfRule type="containsText" dxfId="189" priority="336" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="201" priority="348" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B111)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B306 B296">
-    <cfRule type="containsText" dxfId="188" priority="337" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="200" priority="349" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B296)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B467:B475">
-    <cfRule type="containsText" dxfId="187" priority="334" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="199" priority="346" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B307:B321">
-    <cfRule type="containsText" dxfId="186" priority="335" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="198" priority="347" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B307)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B516">
-    <cfRule type="containsText" dxfId="185" priority="333" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="197" priority="345" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B516)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B450">
-    <cfRule type="containsText" dxfId="184" priority="331" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="196" priority="343" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B449">
-    <cfRule type="containsText" dxfId="183" priority="330" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="195" priority="342" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B322:B448">
-    <cfRule type="containsText" dxfId="182" priority="329" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="194" priority="341" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B322)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G504">
-    <cfRule type="containsText" dxfId="181" priority="309" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="193" priority="321" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G504)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37 C39:C40">
-    <cfRule type="containsText" dxfId="180" priority="304" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="192" priority="316" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E409">
-    <cfRule type="containsText" dxfId="179" priority="302" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="191" priority="314" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E409)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M112:N112">
-    <cfRule type="containsText" dxfId="178" priority="295" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="190" priority="307" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C71:D71">
-    <cfRule type="containsText" dxfId="177" priority="290" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="189" priority="302" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C71)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C92:D92">
-    <cfRule type="containsText" dxfId="176" priority="288" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="188" priority="300" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C92)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C129:D130">
-    <cfRule type="containsText" dxfId="175" priority="263" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="187" priority="275" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",C129)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G126:G130 M126:N130">
-    <cfRule type="containsText" dxfId="174" priority="262" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="186" priority="274" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B169:B171">
-    <cfRule type="containsText" dxfId="173" priority="261" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="185" priority="273" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G169:G170">
-    <cfRule type="containsText" dxfId="172" priority="260" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="184" priority="272" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H169:N170">
-    <cfRule type="containsText" dxfId="171" priority="259" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="183" priority="271" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H169)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M446:N449 M438:N443 M420:N427 M92:N92 M87:N87 M71:N71 M54:N56 M50:N50 M37:N37 M39:N40">
-    <cfRule type="containsText" dxfId="170" priority="257" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="182" priority="269" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M37)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M65:N65 G65">
-    <cfRule type="containsText" dxfId="169" priority="252" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="181" priority="264" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G65)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B64:B65">
-    <cfRule type="containsText" dxfId="168" priority="254" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="180" priority="266" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M64:N64 G64">
-    <cfRule type="containsText" dxfId="167" priority="253" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="179" priority="265" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G64)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B72:B73">
-    <cfRule type="containsText" dxfId="166" priority="248" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="178" priority="260" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M72:N72">
-    <cfRule type="containsText" dxfId="165" priority="250" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="177" priority="262" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M72)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M73:N73">
-    <cfRule type="containsText" dxfId="164" priority="249" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="176" priority="261" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M73)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B96:D107">
-    <cfRule type="containsText" dxfId="163" priority="245" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="175" priority="257" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M96:N107 G96:G107">
-    <cfRule type="containsText" dxfId="162" priority="246" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="174" priority="258" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G96)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M83:N83 G83">
-    <cfRule type="containsText" dxfId="161" priority="231" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="173" priority="243" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G83)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M82:N82 G82">
-    <cfRule type="containsText" dxfId="160" priority="230" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="172" priority="242" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G207:N207">
-    <cfRule type="containsText" dxfId="159" priority="238" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="171" priority="250" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G207)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B146:B147">
-    <cfRule type="containsText" dxfId="158" priority="240" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="170" priority="252" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G146:G147 M146:N147">
-    <cfRule type="containsText" dxfId="157" priority="239" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="169" priority="251" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G146)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B82">
-    <cfRule type="containsText" dxfId="156" priority="232" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="168" priority="244" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B82)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G123 M123:N123">
-    <cfRule type="containsText" dxfId="155" priority="229" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="167" priority="241" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G123)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B140:B141">
-    <cfRule type="containsText" dxfId="154" priority="226" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="166" priority="238" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G140:G141 M140:N141">
-    <cfRule type="containsText" dxfId="153" priority="225" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="165" priority="237" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G140)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B198:B200">
-    <cfRule type="containsText" dxfId="152" priority="176" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="164" priority="188" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B198)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M198:N200 G198:G200">
-    <cfRule type="containsText" dxfId="151" priority="175" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="163" priority="187" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G198)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B255:B258">
-    <cfRule type="containsText" dxfId="150" priority="165" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="162" priority="177" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B255)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B517:B546">
-    <cfRule type="containsText" dxfId="149" priority="162" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="161" priority="174" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B517)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G81">
-    <cfRule type="containsText" dxfId="148" priority="160" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="160" priority="172" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G81)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H171:N171">
-    <cfRule type="containsText" dxfId="147" priority="156" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="159" priority="168" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H171)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F211:N211">
-    <cfRule type="containsText" dxfId="146" priority="154" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="158" priority="166" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F211)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G171">
-    <cfRule type="containsText" dxfId="145" priority="157" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="157" priority="169" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G171)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F231:N249 F255:N256">
-    <cfRule type="containsText" dxfId="144" priority="151" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="156" priority="163" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F231)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M117:N117 G117">
-    <cfRule type="containsText" dxfId="143" priority="150" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="155" priority="162" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G117)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124:D124">
-    <cfRule type="containsText" dxfId="142" priority="149" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="154" priority="161" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G124 M124:N124">
-    <cfRule type="containsText" dxfId="141" priority="148" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="153" priority="160" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F250:N250">
-    <cfRule type="containsText" dxfId="140" priority="147" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="152" priority="159" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F250)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="containsText" dxfId="139" priority="146" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="151" priority="158" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G342">
-    <cfRule type="containsText" dxfId="138" priority="144" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="150" priority="156" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H342">
-    <cfRule type="containsText" dxfId="137" priority="143" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="149" priority="155" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H342)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F340">
-    <cfRule type="containsText" dxfId="136" priority="142" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="148" priority="154" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F350:F366">
-    <cfRule type="containsText" dxfId="135" priority="141" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="147" priority="153" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F350)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I340">
-    <cfRule type="containsText" dxfId="134" priority="140" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="146" priority="152" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J340">
-    <cfRule type="containsText" dxfId="133" priority="139" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="145" priority="151" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K340">
-    <cfRule type="containsText" dxfId="132" priority="138" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="144" priority="150" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L340">
-    <cfRule type="containsText" dxfId="131" priority="137" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="143" priority="149" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M340">
-    <cfRule type="containsText" dxfId="130" priority="136" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="142" priority="148" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N340">
-    <cfRule type="containsText" dxfId="129" priority="135" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="141" priority="147" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H340">
-    <cfRule type="containsText" dxfId="128" priority="134" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="140" priority="146" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H340)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G20:G24 M20:N24">
-    <cfRule type="containsText" dxfId="127" priority="130" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="139" priority="142" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G20)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G457:G465">
-    <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="138" priority="141" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M457:M465">
-    <cfRule type="containsText" dxfId="125" priority="128" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="137" priority="140" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N457:N465">
-    <cfRule type="containsText" dxfId="124" priority="127" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="136" priority="139" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N457)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M593:N593">
-    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="135" priority="138" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M593)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M594:N594">
-    <cfRule type="containsText" dxfId="122" priority="125" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="134" priority="137" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M594)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F341">
-    <cfRule type="containsText" dxfId="121" priority="124" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="133" priority="136" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I341">
-    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="132" priority="135" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J341">
-    <cfRule type="containsText" dxfId="119" priority="122" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="131" priority="134" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K341">
-    <cfRule type="containsText" dxfId="118" priority="121" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="130" priority="133" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L341">
-    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="129" priority="132" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M341">
-    <cfRule type="containsText" dxfId="116" priority="119" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="128" priority="131" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N341">
-    <cfRule type="containsText" dxfId="115" priority="118" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="127" priority="130" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H341">
-    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="126" priority="129" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H341)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E343:F343">
-    <cfRule type="containsText" dxfId="113" priority="116" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="125" priority="128" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",E343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I343">
-    <cfRule type="containsText" dxfId="112" priority="115" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="124" priority="127" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",I343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J343">
-    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="123" priority="126" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",J343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K343">
-    <cfRule type="containsText" dxfId="110" priority="113" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="122" priority="125" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",K343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L343">
-    <cfRule type="containsText" dxfId="109" priority="112" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="121" priority="124" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",L343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M343">
-    <cfRule type="containsText" dxfId="108" priority="111" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="120" priority="123" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N343">
-    <cfRule type="containsText" dxfId="107" priority="110" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="119" priority="122" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",N343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G343">
-    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="118" priority="121" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H343">
-    <cfRule type="containsText" dxfId="105" priority="108" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="117" priority="120" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H343)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H367:N367">
-    <cfRule type="containsText" dxfId="104" priority="107" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="116" priority="119" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H367)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F367">
-    <cfRule type="containsText" dxfId="103" priority="106" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="115" priority="118" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F367)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H368:N368">
-    <cfRule type="containsText" dxfId="102" priority="105" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="114" priority="117" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H368)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F368">
-    <cfRule type="containsText" dxfId="101" priority="104" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="113" priority="116" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F368)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H369:N369">
-    <cfRule type="containsText" dxfId="100" priority="103" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="112" priority="115" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H369)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F369">
-    <cfRule type="containsText" dxfId="99" priority="102" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="111" priority="114" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F369)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H379:N379">
-    <cfRule type="containsText" dxfId="98" priority="100" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="110" priority="112" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H379)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F379">
-    <cfRule type="containsText" dxfId="97" priority="101" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="109" priority="113" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F379)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H380:N384">
-    <cfRule type="containsText" dxfId="96" priority="98" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="108" priority="110" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",H380)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F380:F384">
-    <cfRule type="containsText" dxfId="95" priority="99" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="107" priority="111" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",F380)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M38:N38 G38 A38:C38">
-    <cfRule type="containsText" dxfId="94" priority="97" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="106" priority="109" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A139:N139">
-    <cfRule type="containsText" dxfId="93" priority="92" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="105" priority="104" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A139)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A125 C125:N125">
-    <cfRule type="containsText" dxfId="92" priority="93" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="104" priority="105" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A142:N143">
-    <cfRule type="containsText" dxfId="91" priority="91" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="103" priority="103" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A142)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A172:A176 C172:N176">
-    <cfRule type="containsText" dxfId="90" priority="90" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="102" priority="102" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A177:A196 C177:N196">
-    <cfRule type="containsText" dxfId="89" priority="89" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="101" priority="101" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A177)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A251:N254">
-    <cfRule type="containsText" dxfId="88" priority="88" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="100" priority="100" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A251)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M640:N640">
-    <cfRule type="containsText" dxfId="87" priority="39" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="99" priority="51" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",M640)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A261 H261:N261 C261:F261">
-    <cfRule type="containsText" dxfId="86" priority="86" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="98" priority="98" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G447">
-    <cfRule type="containsText" dxfId="85" priority="84" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="97" priority="96" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G447)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G447">
-    <cfRule type="containsText" dxfId="84" priority="85" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="96" priority="97" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G447)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G448">
-    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="95" priority="94" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G448)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G448">
-    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="94" priority="95" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G448)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G449">
-    <cfRule type="containsText" dxfId="81" priority="80" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="93" priority="92" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G449">
-    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="92" priority="93" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G449)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G450">
-    <cfRule type="containsText" dxfId="79" priority="78" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="91" priority="90" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G450">
-    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="90" priority="91" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G450)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G451">
-    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="89" priority="88" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G451)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G451">
-    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="88" priority="89" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G451)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G452">
-    <cfRule type="containsText" dxfId="75" priority="74" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="87" priority="86" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G452)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G452">
-    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="86" priority="87" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G452)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G453">
-    <cfRule type="containsText" dxfId="73" priority="72" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="85" priority="84" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G453)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G453">
-    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="84" priority="85" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G453)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G454">
-    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="83" priority="82" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G454)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G454">
-    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="82" priority="83" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G454)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G455">
-    <cfRule type="containsText" dxfId="69" priority="68" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="81" priority="80" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G455">
-    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="80" priority="81" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G455)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G466">
-    <cfRule type="containsText" dxfId="67" priority="66" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="79" priority="78" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G466">
-    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="78" priority="79" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G466)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G467">
-    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="77" priority="76" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G467">
-    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="76" priority="77" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G467)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G468">
-    <cfRule type="containsText" dxfId="63" priority="62" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="75" priority="74" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G468)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G468">
-    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="74" priority="75" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G468)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G469">
-    <cfRule type="containsText" dxfId="61" priority="60" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="73" priority="72" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G469)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G469">
-    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="72" priority="73" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G469)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G470">
-    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="71" priority="70" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G470)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G470">
-    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="70" priority="71" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G470)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G471">
-    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="69" priority="68" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G471)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G471">
-    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="68" priority="69" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G471)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G472">
-    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="67" priority="66" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G472)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G472">
-    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="66" priority="67" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G472)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G473">
-    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="65" priority="64" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G473)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G473">
-    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="64" priority="65" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G473)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G474">
-    <cfRule type="containsText" dxfId="51" priority="50" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="63" priority="62" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G474)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G474">
-    <cfRule type="containsText" dxfId="50" priority="51" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="62" priority="63" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G474)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G475">
-    <cfRule type="containsText" dxfId="49" priority="48" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="61" priority="60" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G475)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G475">
-    <cfRule type="containsText" dxfId="48" priority="49" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="60" priority="61" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G475)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G476">
-    <cfRule type="containsText" dxfId="47" priority="46" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="59" priority="58" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G476)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G476">
-    <cfRule type="containsText" dxfId="46" priority="47" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="58" priority="59" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G476)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G477">
-    <cfRule type="containsText" dxfId="45" priority="44" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="57" priority="56" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G477)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G477">
-    <cfRule type="containsText" dxfId="44" priority="45" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="56" priority="57" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G477)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G478">
-    <cfRule type="containsText" dxfId="43" priority="42" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="55" priority="54" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G478)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G478">
-    <cfRule type="containsText" dxfId="42" priority="43" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="54" priority="55" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G478)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G479">
-    <cfRule type="containsText" dxfId="41" priority="40" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="53" priority="52" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G479)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G479">
-    <cfRule type="containsText" dxfId="40" priority="41" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="52" priority="53" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G479)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31:G36 G25:G28 B25:C36 M25:N36">
-    <cfRule type="containsText" dxfId="39" priority="37" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="51" priority="49" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B25)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G29:G30">
-    <cfRule type="containsText" dxfId="38" priority="38" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="50" priority="50" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G29)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4 M4:N4 A4:C4">
-    <cfRule type="containsText" dxfId="37" priority="34" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="49" priority="46" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O90 O92:O670">
-    <cfRule type="containsText" dxfId="36" priority="32" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="48" priority="44" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",O2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G3 B2:C3 M2:N3">
-    <cfRule type="containsText" dxfId="35" priority="33" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="47" priority="45" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G261">
-    <cfRule type="containsText" dxfId="34" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="46" priority="43" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A91:G91 O91">
-    <cfRule type="containsText" dxfId="33" priority="30" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="45" priority="42" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A91)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B261">
-    <cfRule type="containsText" dxfId="32" priority="29" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="44" priority="41" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B261)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B515">
-    <cfRule type="containsText" dxfId="31" priority="28" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="43" priority="40" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B515)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M515:N515 G515">
-    <cfRule type="containsText" dxfId="30" priority="27" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="42" priority="39" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",G515)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:B196">
-    <cfRule type="containsText" dxfId="29" priority="24" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="41" priority="36" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B172:B196">
-    <cfRule type="containsText" dxfId="28" priority="25" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="40" priority="37" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B172)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:B63">
-    <cfRule type="containsText" dxfId="23" priority="23" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="35" priority="35" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A108:B108">
-    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="33" priority="34" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B108:C108">
-    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="32" priority="33" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B108)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B109">
-    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="31" priority="32" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B109)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B110">
-    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="30" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B110)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B112">
-    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="29" priority="30" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B112)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B113">
-    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="28" priority="29" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B113)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B114">
-    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="27" priority="28" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B114)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="26" priority="27" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B115">
-    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="25" priority="26" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B115)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A119:B119">
-    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="24" priority="25" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B119">
-    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B119)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="22" priority="23" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B122">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="21" priority="22" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B122)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="20" priority="21" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B124">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="19" priority="20" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B124)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="17" priority="18" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125">
-    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="16" priority="17" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B125">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="15" priority="16" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B125)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B126">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="14" priority="15" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B126">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="13" priority="14" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B126)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B126">
+    <cfRule type="containsText" dxfId="12" priority="13" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B126)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B129">
+    <cfRule type="containsText" dxfId="11" priority="12" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B129)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B129">
+    <cfRule type="containsText" dxfId="10" priority="11" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B129)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B129">
+    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B129)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B130">
+    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B130)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B130">
+    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B130)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B130">
+    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B130)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B131">
+    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B131)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B131">
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B131)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B131">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B131)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B132">
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B132)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B132">
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="&lt;?&gt;">
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B132)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B132">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="&lt;?&gt;">
-      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B126)))</formula>
+      <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",B132)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -45585,7 +45765,7 @@
   </sheetData>
   <autoFilter ref="A1:B1" xr:uid="{AF62FD2E-052D-40DF-8032-68688A8C1623}"/>
   <conditionalFormatting sqref="A2:B479">
-    <cfRule type="containsText" dxfId="27" priority="2" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="39" priority="2" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -45915,12 +46095,12 @@
     <mergeCell ref="A1:B1"/>
   </mergeCells>
   <conditionalFormatting sqref="A1 C1 A2:C37 A39:C1048576">
-    <cfRule type="containsText" dxfId="26" priority="31" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="38" priority="31" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A38:C38">
-    <cfRule type="containsText" dxfId="25" priority="6" operator="containsText" text="&lt;?&gt;">
+    <cfRule type="containsText" dxfId="37" priority="6" operator="containsText" text="&lt;?&gt;">
       <formula>NOT(ISERROR(SEARCH("&lt;?&gt;",A38)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
overbodige activiteit uit ow bestanden verwijderd
</commit_message>
<xml_diff>
--- a/1.0.4/matrix/Validatiematrix v1.2.xlsx
+++ b/1.0.4/matrix/Validatiematrix v1.2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_validatietestcontent\1.0.4\matrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717F12C2-FE86-4BE0-A07B-2B855CA7D967}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F6E4264-11F4-4767-B1E4-9ACDF8F951A1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" tabRatio="670" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9621,7 +9621,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A430" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C444" sqref="C444"/>
+      <selection pane="bottomLeft" activeCell="A434" sqref="A434"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -30264,7 +30264,7 @@
       </c>
     </row>
     <row r="431" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A431" s="38" t="s">
+      <c r="A431" s="74" t="s">
         <v>1166</v>
       </c>
       <c r="B431" s="79">
@@ -30312,7 +30312,7 @@
       </c>
     </row>
     <row r="432" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A432" s="38" t="s">
+      <c r="A432" s="74" t="s">
         <v>1166</v>
       </c>
       <c r="B432" s="79">
@@ -30600,7 +30600,7 @@
       </c>
     </row>
     <row r="438" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A438" s="38" t="s">
+      <c r="A438" s="74" t="s">
         <v>1166</v>
       </c>
       <c r="B438" s="79">
@@ -30648,7 +30648,7 @@
       </c>
     </row>
     <row r="439" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A439" s="38" t="s">
+      <c r="A439" s="74" t="s">
         <v>1166</v>
       </c>
       <c r="B439" s="79">
@@ -31272,7 +31272,7 @@
       </c>
     </row>
     <row r="452" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A452" s="38" t="s">
+      <c r="A452" s="74" t="s">
         <v>1166</v>
       </c>
       <c r="B452" s="79">
@@ -31320,7 +31320,7 @@
       </c>
     </row>
     <row r="453" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A453" s="38" t="s">
+      <c r="A453" s="74" t="s">
         <v>1166</v>
       </c>
       <c r="B453" s="79">
@@ -31464,7 +31464,7 @@
       </c>
     </row>
     <row r="456" spans="1:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A456" s="38" t="s">
+      <c r="A456" s="74" t="s">
         <v>1166</v>
       </c>
       <c r="B456" s="79">

</xml_diff>